<commit_message>
T-174: - nuevos atributos en la entity ModelBrandEntity y nueva tabla para guardar los tipos de cargadores de los modelos
</commit_message>
<xml_diff>
--- a/modelos.xlsx
+++ b/modelos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="121">
   <si>
     <t xml:space="preserve">Audi</t>
   </si>
@@ -437,40 +437,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FFD9D9E3"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFD9D9E3"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFD9D9E3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFD9D9E3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin">
-        <color rgb="FFD9D9E3"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFD9D9E3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFD9D9E3"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -523,8 +495,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -533,14 +509,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -623,1126 +591,1093 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="n">
+      <c r="C1" s="1" t="n">
         <v>328</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="n">
+      <c r="C2" s="1" t="n">
         <v>472</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C3" s="1" t="n">
         <v>482</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C4" s="1" t="n">
         <v>328</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="n">
+      <c r="C5" s="1" t="n">
         <v>520</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="n">
+      <c r="C6" s="1" t="n">
         <v>310</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4" t="n">
+      <c r="C7" s="1" t="n">
         <v>630</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4" t="n">
+      <c r="C8" s="1" t="n">
         <v>459</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="4" t="n">
+      <c r="C9" s="1" t="n">
         <v>322</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="4" t="n">
+      <c r="C10" s="1" t="n">
         <v>322</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="4" t="n">
+      <c r="C11" s="1" t="n">
         <v>360</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="4" t="n">
+      <c r="C12" s="1" t="n">
         <v>520</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="4" t="n">
+      <c r="C13" s="1" t="n">
         <v>370</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="4" t="n">
+      <c r="C14" s="1" t="n">
         <v>402</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="4" t="n">
+      <c r="C15" s="1" t="n">
         <v>416</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="4" t="n">
+      <c r="C16" s="1" t="n">
         <v>350</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="4" t="n">
+      <c r="C17" s="1" t="n">
         <v>320</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="4" t="n">
+      <c r="C18" s="1" t="n">
         <v>804</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="4" t="n">
+      <c r="C19" s="1" t="n">
         <v>378</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="4" t="n">
+      <c r="C20" s="1" t="n">
         <v>608</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="4" t="n">
+      <c r="C21" s="1" t="n">
         <v>480</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="4" t="n">
+      <c r="C22" s="1" t="n">
         <v>350</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="4" t="n">
+      <c r="C23" s="1" t="n">
         <v>329</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="4" t="n">
+      <c r="C24" s="1" t="n">
         <v>480</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="4" t="n">
+      <c r="C25" s="1" t="n">
         <v>483</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="4" t="n">
+      <c r="C26" s="1" t="n">
         <v>480</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="4" t="n">
+      <c r="C27" s="1" t="n">
         <v>427</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="4" t="n">
+      <c r="C28" s="1" t="n">
         <v>560</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="4" t="n">
+      <c r="C29" s="1" t="n">
         <v>480</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="4" t="n">
+      <c r="C30" s="1" t="n">
         <v>484</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="4" t="n">
+      <c r="C31" s="1" t="n">
         <v>470</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="4" t="n">
+      <c r="C32" s="1" t="n">
         <v>510</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="s">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="4" t="n">
+      <c r="C33" s="1" t="n">
         <v>455</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="4" t="n">
+      <c r="C34" s="1" t="n">
         <v>386</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="s">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="4" t="n">
+      <c r="C35" s="1" t="n">
         <v>300</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="s">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="4" t="n">
+      <c r="C36" s="1" t="n">
         <v>400</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="s">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="4" t="n">
+      <c r="C37" s="1" t="n">
         <v>832</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="s">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="4" t="n">
+      <c r="C38" s="1" t="n">
         <v>834</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="s">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="4" t="n">
+      <c r="C39" s="1" t="n">
         <v>832</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="s">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="4" t="n">
+      <c r="C40" s="1" t="n">
         <v>832</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="4" t="n">
+      <c r="C41" s="1" t="n">
         <v>800</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="s">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C42" s="4" t="n">
+      <c r="C42" s="1" t="n">
         <v>200</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="4" t="n">
+      <c r="C43" s="1" t="n">
         <v>424</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="4" t="n">
+      <c r="C44" s="1" t="n">
         <v>419</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="s">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="4" t="n">
+      <c r="C45" s="1" t="n">
         <v>355</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="s">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="4" t="n">
+      <c r="C46" s="1" t="n">
         <v>660</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="s">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="4" t="n">
+      <c r="C47" s="1" t="n">
         <v>770</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="3" t="s">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="4" t="n">
+      <c r="C48" s="1" t="n">
         <v>358</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="3" t="s">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C49" s="4" t="n">
+      <c r="C49" s="1" t="n">
         <v>400</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="3" t="s">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C50" s="4" t="n">
+      <c r="C50" s="1" t="n">
         <v>263</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="s">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="4" t="n">
+      <c r="C51" s="1" t="n">
         <v>232</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="s">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="4" t="n">
+      <c r="C52" s="1" t="n">
         <v>234</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3" t="s">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C53" s="4" t="n">
+      <c r="C53" s="1" t="n">
         <v>580</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="3" t="s">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C54" s="4" t="n">
+      <c r="C54" s="1" t="n">
         <v>580</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="3" t="s">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C55" s="4" t="n">
+      <c r="C55" s="1" t="n">
         <v>610</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3" t="s">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C56" s="4" t="n">
+      <c r="C56" s="1" t="n">
         <v>270</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="3" t="s">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C57" s="4" t="n">
+      <c r="C57" s="1" t="n">
         <v>385</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="3" t="s">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C58" s="4" t="n">
+      <c r="C58" s="1" t="n">
         <v>337</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3" t="s">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C59" s="4" t="n">
+      <c r="C59" s="1" t="n">
         <v>310</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="3" t="s">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C60" s="4" t="n">
+      <c r="C60" s="1" t="n">
         <v>340</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3" t="s">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B61" s="4" t="n">
+      <c r="B61" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C61" s="4" t="n">
+      <c r="C61" s="1" t="n">
         <v>480</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="3" t="s">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B62" s="4" t="n">
+      <c r="B62" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C62" s="4" t="n">
+      <c r="C62" s="1" t="n">
         <v>470</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="3" t="s">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B63" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C63" s="4" t="n">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="3" t="s">
+      <c r="B63" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C63" s="1" t="n">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B64" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C64" s="4" t="n">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B65" s="4" t="s">
+      <c r="B64" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C65" s="4" t="n">
+      <c r="C64" s="1" t="n">
         <v>804</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="3" t="s">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B65" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C66" s="4" t="n">
+      <c r="C65" s="1" t="n">
         <v>408</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="3" t="s">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B67" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C67" s="4" t="n">
+      <c r="B66" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C66" s="1" t="n">
         <v>408</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C68" s="4" t="n">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3" t="s">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B67" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C69" s="4" t="n">
+      <c r="C67" s="1" t="n">
         <v>395</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="3" t="s">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B68" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C70" s="4" t="n">
+      <c r="C68" s="1" t="n">
         <v>650</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3" t="s">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B69" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C71" s="4" t="n">
+      <c r="C69" s="1" t="n">
         <v>483</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="3" t="s">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B70" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C72" s="4" t="n">
+      <c r="C70" s="1" t="n">
         <v>483</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="3" t="s">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B73" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C73" s="4" t="n">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B74" s="4" t="s">
+      <c r="B71" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C74" s="4" t="n">
+      <c r="C71" s="1" t="n">
         <v>643</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="3" t="s">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B72" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C75" s="4" t="n">
+      <c r="C72" s="1" t="n">
         <v>537</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="3" t="s">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B73" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C76" s="4" t="n">
+      <c r="C73" s="1" t="n">
         <v>130</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="3" t="s">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B74" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C77" s="4" t="n">
+      <c r="C74" s="1" t="n">
         <v>127</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3" t="s">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B75" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C78" s="4" t="n">
+      <c r="C75" s="1" t="n">
         <v>800</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3" t="s">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B76" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C79" s="4" t="n">
+      <c r="C76" s="1" t="n">
         <v>523</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3" t="s">
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B77" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C80" s="4" t="n">
+      <c r="C77" s="1" t="n">
         <v>580</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3" t="s">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B78" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C81" s="4" t="n">
+      <c r="C78" s="1" t="n">
         <v>567</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="3" t="s">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B79" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C82" s="4" t="n">
+      <c r="C79" s="1" t="n">
         <v>448</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="3" t="s">
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B80" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C83" s="4" t="n">
+      <c r="C80" s="1" t="n">
         <v>610</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="3" t="s">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B81" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C84" s="4" t="n">
+      <c r="C81" s="1" t="n">
         <v>628</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="3" t="s">
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B82" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C85" s="4" t="n">
+      <c r="C82" s="1" t="n">
         <v>565</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="3" t="s">
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B83" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C86" s="4" t="n">
+      <c r="C83" s="1" t="n">
         <v>547</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="3" t="s">
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B84" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C87" s="4" t="n">
+      <c r="C84" s="1" t="n">
         <v>505</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="3" t="s">
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B85" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C88" s="4" t="n">
+      <c r="C85" s="1" t="n">
         <v>505</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="3" t="s">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B86" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C89" s="4" t="n">
+      <c r="C86" s="1" t="n">
         <v>468</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="3" t="s">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B87" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C90" s="4" t="n">
+      <c r="C87" s="1" t="n">
         <v>1000</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="3" t="s">
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B88" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C91" s="4" t="n">
+      <c r="C88" s="1" t="n">
         <v>342</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="3" t="s">
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B89" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C92" s="4" t="n">
+      <c r="C89" s="1" t="n">
         <v>424</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="3" t="s">
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B90" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C93" s="4" t="n">
+      <c r="C90" s="1" t="n">
         <v>520</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="3" t="s">
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B91" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C94" s="4" t="n">
+      <c r="C91" s="1" t="n">
         <v>480</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3" t="s">
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B92" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C95" s="4" t="n">
+      <c r="C92" s="1" t="n">
         <v>588</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="3"/>
-      <c r="B96" s="4"/>
-      <c r="C96" s="4"/>
-    </row>
-    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="3"/>
-      <c r="B97" s="4"/>
-      <c r="C97" s="4"/>
-    </row>
-    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="3"/>
-      <c r="B98" s="4"/>
-      <c r="C98" s="4"/>
-    </row>
-    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="3"/>
-      <c r="B99" s="4"/>
-      <c r="C99" s="4"/>
-    </row>
-    <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="3"/>
-      <c r="B100" s="4"/>
-      <c r="C100" s="4"/>
-    </row>
-    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="3"/>
-      <c r="B101" s="4"/>
-      <c r="C101" s="4"/>
-    </row>
-    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="3"/>
-      <c r="B102" s="4"/>
-      <c r="C102" s="4"/>
-    </row>
-    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="3"/>
-      <c r="B103" s="4"/>
-      <c r="C103" s="4"/>
-    </row>
-    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="3"/>
-      <c r="B104" s="4"/>
-      <c r="C104" s="4"/>
-    </row>
-    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="3"/>
-      <c r="B105" s="4"/>
-      <c r="C105" s="4"/>
-    </row>
-    <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="3"/>
-      <c r="B106" s="4"/>
-      <c r="C106" s="4"/>
-    </row>
-    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="3"/>
-      <c r="B107" s="4"/>
-      <c r="C107" s="4"/>
-    </row>
-    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="3"/>
-      <c r="B108" s="4"/>
-      <c r="C108" s="4"/>
-    </row>
-    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="3"/>
-      <c r="B109" s="4"/>
-      <c r="C109" s="4"/>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="2"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="2"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="2"/>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="2"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="2"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="2"/>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="2"/>
+      <c r="B102" s="3"/>
+      <c r="C102" s="3"/>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="2"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="2"/>
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="2"/>
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="2"/>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="2"/>
+      <c r="B107" s="3"/>
+      <c r="C107" s="3"/>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="2"/>
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>